<commit_message>
Changed some language translations. Updated travel-expense route and template document to not skip rows (i.e. when selecting only mondays, only tuesdays etc.)
</commit_message>
<xml_diff>
--- a/templates/Honorari.xlsx
+++ b/templates/Honorari.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\admin\admin\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB79457-D329-405C-996A-45DE1EF4AE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB65046F-1409-4568-8EB4-FE142DDC66A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
     <t>Adresa rada</t>
   </si>
   <si>
-    <t>Ime ustanove</t>
+    <t>Srednja škola Ilok</t>
   </si>
 </sst>
 </file>
@@ -276,14 +276,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -292,22 +303,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalno" xfId="0" builtinId="0"/>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="V26" sqref="V26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,119 +641,119 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="J3" s="19" t="s">
+      <c r="B3" s="6"/>
+      <c r="J3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="G4" s="8" t="s">
+      <c r="B4" s="6"/>
+      <c r="G4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7"/>
-      <c r="K5" s="18" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="K5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
     </row>
     <row r="9" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AC9" s="13"/>
+      <c r="AC9" s="16"/>
     </row>
     <row r="10" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="1">
         <v>2</v>
       </c>
@@ -822,41 +822,41 @@
       </c>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
-      <c r="AB10" s="14"/>
-      <c r="AC10" s="15"/>
+      <c r="AB10" s="17"/>
+      <c r="AC10" s="18"/>
     </row>
     <row r="11" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="5" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
       <c r="AA11" s="4"/>
-      <c r="AB11" s="16"/>
-      <c r="AC11" s="17"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="20"/>
     </row>
     <row r="12" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1110,64 +1110,54 @@
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="12"/>
       <c r="AA20" s="4"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="4"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="J23" s="7" t="s">
+      <c r="J23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="X23" s="7" t="s">
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="X23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Y23" s="7"/>
-      <c r="Z23" s="7"/>
-      <c r="AA23" s="7"/>
-      <c r="AB23" s="7"/>
-      <c r="AC23" s="7"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="G4:R4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="D9:AA9"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D11:AA11"/>
-    <mergeCell ref="F7:V7"/>
     <mergeCell ref="AB17:AC17"/>
     <mergeCell ref="AB18:AC18"/>
     <mergeCell ref="B20:AA20"/>
@@ -1184,6 +1174,16 @@
     <mergeCell ref="AB19:AC19"/>
     <mergeCell ref="AB13:AC13"/>
     <mergeCell ref="AB9:AC11"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="G4:R4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="D9:AA9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D11:AA11"/>
+    <mergeCell ref="F7:V7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated DB to include two more properties in settings (organisation name and ticket price). Reworked all routes and templates to include these properties.
</commit_message>
<xml_diff>
--- a/templates/Honorari.xlsx
+++ b/templates/Honorari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\admin\admin\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB65046F-1409-4568-8EB4-FE142DDC66A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7746B83-2288-4655-BF85-B2E3D4955A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>za održane honorarne sate u mjesecu</t>
   </si>
   <si>
-    <t xml:space="preserve">Prezime i ime učitelja - nastavnika: </t>
-  </si>
-  <si>
     <t>PREDMET</t>
   </si>
   <si>
@@ -78,7 +75,10 @@
     <t>Adresa rada</t>
   </si>
   <si>
-    <t>Srednja škola Ilok</t>
+    <t>Naziv organizacije</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ime i prezime učitelja - nastavnika: </t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <dimension ref="A3:AC23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
   <sheetData>
     <row r="3" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6"/>
       <c r="J3" s="11" t="s">
@@ -656,7 +656,7 @@
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="6"/>
       <c r="G4" s="5" t="s">
@@ -678,7 +678,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="K5" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
@@ -686,7 +686,7 @@
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -711,16 +711,16 @@
     </row>
     <row r="9" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="C9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="D9" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>6</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
@@ -746,7 +746,7 @@
       <c r="Z9" s="12"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AC9" s="16"/>
     </row>
@@ -830,7 +830,7 @@
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="20" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="12"/>
@@ -1141,14 +1141,14 @@
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J23" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="X23" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y23" s="6"/>
       <c r="Z23" s="6"/>

</xml_diff>